<commit_message>
Zeitplan auf neuer Termin angepasst
</commit_message>
<xml_diff>
--- a/Zeitplan.xlsx
+++ b/Zeitplan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Schule\Modul_306_IT_Kleinprojekt_entwickeln\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Schule\Modul_306_IT_Kleinprojekt_entwickeln\Webseite_Modul_306\Modul-306\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71965B3D-1176-4C4B-946E-4036D481AFB9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DAA9B21-0B5C-448A-A211-52AB840B8722}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{76173DC6-1BEA-4CBB-95AA-806EA72F933C}"/>
   </bookViews>
@@ -108,9 +108,6 @@
     <t>Projekt Abgabe</t>
   </si>
   <si>
-    <t>Projekt im Classroom einreichen bis 13.10.2019, 23:59</t>
-  </si>
-  <si>
     <t>Projekt fertigstellen</t>
   </si>
   <si>
@@ -127,6 +124,9 @@
   </si>
   <si>
     <t>Pflichtenheft v1.00</t>
+  </si>
+  <si>
+    <t>Projekt im Classroom einreichen bis 20.10.2019, 23:59</t>
   </si>
 </sst>
 </file>
@@ -550,13 +550,13 @@
                   <c:v>43741</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43747</c:v>
+                  <c:v>43750</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43748</c:v>
+                  <c:v>43757</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43751</c:v>
+                  <c:v>43758</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -798,10 +798,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1</c:v>
@@ -810,7 +810,7 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>1</c:v>
@@ -889,7 +889,7 @@
         <c:axId val="558752048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="43752"/>
+          <c:max val="43759"/>
           <c:min val="43699"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1527,15 +1527,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>99060</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>708660</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1862,8 +1862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74034589-8F6D-4899-B880-E4AC87FEE608}">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1924,7 +1924,7 @@
         <v>43699</v>
       </c>
       <c r="E4" s="12">
-        <f t="shared" ref="E4:E16" si="0">D4+C4</f>
+        <f t="shared" ref="E4:E14" si="0">D4+C4</f>
         <v>43706</v>
       </c>
       <c r="F4" s="1"/>
@@ -2007,10 +2007,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" s="10">
         <v>1</v>
@@ -2029,14 +2029,14 @@
         <v>17</v>
       </c>
       <c r="C10" s="10">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D10" s="11">
         <v>43720</v>
       </c>
       <c r="E10" s="12">
         <f>D10+C10</f>
-        <v>43740</v>
+        <v>43750</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -2047,22 +2047,22 @@
         <v>19</v>
       </c>
       <c r="C11" s="10">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D11" s="11">
         <v>43720</v>
       </c>
       <c r="E11" s="12">
         <f>D11+C11</f>
-        <v>43740</v>
+        <v>43750</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="13" t="s">
         <v>28</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>29</v>
       </c>
       <c r="C12" s="10">
         <v>1</v>
@@ -2098,28 +2098,28 @@
         <v>23</v>
       </c>
       <c r="C14" s="10">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D14" s="11">
-        <v>43747</v>
+        <v>43750</v>
       </c>
       <c r="E14" s="12">
         <f t="shared" si="0"/>
-        <v>43750</v>
+        <v>43756</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>26</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>27</v>
       </c>
       <c r="C15" s="10">
         <v>1</v>
       </c>
       <c r="D15" s="11">
-        <v>43748</v>
+        <v>43757</v>
       </c>
       <c r="E15" s="12"/>
     </row>
@@ -2128,13 +2128,13 @@
         <v>24</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C16" s="16">
         <v>1</v>
       </c>
       <c r="D16" s="17">
-        <v>43751</v>
+        <v>43758</v>
       </c>
       <c r="E16" s="18"/>
     </row>

</xml_diff>